<commit_message>
started working on GSR pull module
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaayem\Documents\Python\Kym\Mongo_Search\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaaye\Documents\Python\Kym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC480A72-260C-4D15-816F-95E4EED38875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268EB2CC-8E89-4043-92E5-8DF9C495F82C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{50ED4C38-B0C0-4F98-BDF2-F7ADD0C76675}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50ED4C38-B0C0-4F98-BDF2-F7ADD0C76675}"/>
   </bookViews>
   <sheets>
     <sheet name="GSR" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>code</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>C:\Users\Kaayem\Documents\3. Kaayem\personal\Projects\Python\Python Output</t>
+  </si>
+  <si>
+    <t>rowstart</t>
+  </si>
+  <si>
+    <t>colstart</t>
+  </si>
+  <si>
+    <t>sheetname</t>
+  </si>
+  <si>
+    <t>C:/Users/Kaaye/Documents/Python/Kym/GSRreader/FinalAUABM.xlsm</t>
+  </si>
+  <si>
+    <t>stpath</t>
   </si>
 </sst>
 </file>
@@ -448,14 +463,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D85920-DDC0-4D8B-82D0-9378FB38E333}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -464,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9998BA-82BE-4420-9106-1BA0D03E5910}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>